<commit_message>
back up of current paper data
</commit_message>
<xml_diff>
--- a/RModel/FakeData_desc.xlsx
+++ b/RModel/FakeData_desc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28040" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="conjoints" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>Savings in 25 years</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>Consumer Reports Rating</t>
-  </si>
-  <si>
-    <t>Enegry Cost Savings</t>
   </si>
   <si>
     <t>9 acres of forest</t>
@@ -251,8 +248,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -296,7 +295,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -315,6 +314,7 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -333,6 +333,7 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -664,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -677,39 +678,39 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <f>B2/100</f>
@@ -736,127 +737,127 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B23" s="1">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -887,7 +888,7 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -908,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -929,7 +930,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -950,7 +951,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -976,7 +977,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -997,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1022,17 +1023,16 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>